<commit_message>
Can now handle ####-### format bins
</commit_message>
<xml_diff>
--- a/_LAYOUT.xlsx
+++ b/_LAYOUT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\BinSorting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\BinSortSequence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5104B7D-F89F-49E4-837A-8497768DE68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD963D67-659A-492D-9139-3938F5E85F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4484" uniqueCount="4379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4517" uniqueCount="4410">
   <si>
     <t>01-001-1</t>
   </si>
@@ -13172,6 +13172,99 @@
   </si>
   <si>
     <t>28-252-1</t>
+  </si>
+  <si>
+    <t>LaneSingle.0.0.9000</t>
+  </si>
+  <si>
+    <t>9020-001</t>
+  </si>
+  <si>
+    <t>9020-003</t>
+  </si>
+  <si>
+    <t>9020-005</t>
+  </si>
+  <si>
+    <t>9020-007</t>
+  </si>
+  <si>
+    <t>9020-009</t>
+  </si>
+  <si>
+    <t>9020-002</t>
+  </si>
+  <si>
+    <t>9020-004</t>
+  </si>
+  <si>
+    <t>9020-006</t>
+  </si>
+  <si>
+    <t>9020-008</t>
+  </si>
+  <si>
+    <t>9020-010</t>
+  </si>
+  <si>
+    <t>0104-001</t>
+  </si>
+  <si>
+    <t>0104-002</t>
+  </si>
+  <si>
+    <t>0104-003</t>
+  </si>
+  <si>
+    <t>0104-004</t>
+  </si>
+  <si>
+    <t>0104-005</t>
+  </si>
+  <si>
+    <t>0104-006</t>
+  </si>
+  <si>
+    <t>0104-007</t>
+  </si>
+  <si>
+    <t>0104-008</t>
+  </si>
+  <si>
+    <t>0104-009</t>
+  </si>
+  <si>
+    <t>0104-010</t>
+  </si>
+  <si>
+    <t>9010-001</t>
+  </si>
+  <si>
+    <t>9010-002</t>
+  </si>
+  <si>
+    <t>9010-003</t>
+  </si>
+  <si>
+    <t>9010-004</t>
+  </si>
+  <si>
+    <t>9010-005</t>
+  </si>
+  <si>
+    <t>9010-006</t>
+  </si>
+  <si>
+    <t>9010-007</t>
+  </si>
+  <si>
+    <t>9010-008</t>
+  </si>
+  <si>
+    <t>9010-009</t>
+  </si>
+  <si>
+    <t>9010-010</t>
   </si>
 </sst>
 </file>
@@ -14041,10 +14134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC127"/>
+  <dimension ref="A1:BF127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BC7" sqref="BC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14078,10 +14171,11 @@
     <col min="50" max="51" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="53" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="54" max="55" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="16384" width="9.140625" style="1"/>
+    <col min="56" max="57" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2821</v>
       </c>
@@ -14247,8 +14341,17 @@
       <c r="BC1" s="1" t="s">
         <v>2822</v>
       </c>
+      <c r="BD1" s="1" t="s">
+        <v>4379</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>4379</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>4379</v>
+      </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -14414,8 +14517,17 @@
       <c r="BC2" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="BD2" s="1" t="s">
+        <v>4390</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>4400</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>4380</v>
+      </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -14581,8 +14693,17 @@
       <c r="BC3" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="BD3" s="1" t="s">
+        <v>4391</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>4401</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>4385</v>
+      </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>110</v>
       </c>
@@ -14748,8 +14869,17 @@
       <c r="BC4" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="BD4" s="1" t="s">
+        <v>4392</v>
+      </c>
+      <c r="BE4" s="1" t="s">
+        <v>4402</v>
+      </c>
+      <c r="BF4" s="1" t="s">
+        <v>4381</v>
+      </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>165</v>
       </c>
@@ -14915,8 +15045,17 @@
       <c r="BC5" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="BD5" s="1" t="s">
+        <v>4393</v>
+      </c>
+      <c r="BE5" s="1" t="s">
+        <v>4403</v>
+      </c>
+      <c r="BF5" s="1" t="s">
+        <v>4386</v>
+      </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>220</v>
       </c>
@@ -15082,8 +15221,17 @@
       <c r="BC6" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="BD6" s="1" t="s">
+        <v>4394</v>
+      </c>
+      <c r="BE6" s="1" t="s">
+        <v>4404</v>
+      </c>
+      <c r="BF6" s="1" t="s">
+        <v>4382</v>
+      </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>275</v>
       </c>
@@ -15249,8 +15397,17 @@
       <c r="BC7" s="1" t="s">
         <v>329</v>
       </c>
+      <c r="BD7" s="1" t="s">
+        <v>4395</v>
+      </c>
+      <c r="BE7" s="1" t="s">
+        <v>4405</v>
+      </c>
+      <c r="BF7" s="1" t="s">
+        <v>4387</v>
+      </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>330</v>
       </c>
@@ -15416,8 +15573,17 @@
       <c r="BC8" s="1" t="s">
         <v>384</v>
       </c>
+      <c r="BD8" s="1" t="s">
+        <v>4396</v>
+      </c>
+      <c r="BE8" s="1" t="s">
+        <v>4406</v>
+      </c>
+      <c r="BF8" s="1" t="s">
+        <v>4383</v>
+      </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>385</v>
       </c>
@@ -15583,8 +15749,17 @@
       <c r="BC9" s="1" t="s">
         <v>439</v>
       </c>
+      <c r="BD9" s="1" t="s">
+        <v>4397</v>
+      </c>
+      <c r="BE9" s="1" t="s">
+        <v>4407</v>
+      </c>
+      <c r="BF9" s="1" t="s">
+        <v>4388</v>
+      </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>440</v>
       </c>
@@ -15750,8 +15925,17 @@
       <c r="BC10" s="1" t="s">
         <v>494</v>
       </c>
+      <c r="BD10" s="1" t="s">
+        <v>4398</v>
+      </c>
+      <c r="BE10" s="1" t="s">
+        <v>4408</v>
+      </c>
+      <c r="BF10" s="1" t="s">
+        <v>4384</v>
+      </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>495</v>
       </c>
@@ -15917,8 +16101,17 @@
       <c r="BC11" s="1" t="s">
         <v>549</v>
       </c>
+      <c r="BD11" s="1" t="s">
+        <v>4399</v>
+      </c>
+      <c r="BE11" s="1" t="s">
+        <v>4409</v>
+      </c>
+      <c r="BF11" s="1" t="s">
+        <v>4389</v>
+      </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>550</v>
       </c>
@@ -16085,7 +16278,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>605</v>
       </c>
@@ -16252,7 +16445,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>660</v>
       </c>
@@ -16419,7 +16612,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>715</v>
       </c>
@@ -16586,7 +16779,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>770</v>
       </c>

</xml_diff>

<commit_message>
Updated for SRTUP seq_no limitation(99999) and Timeout issue.
</commit_message>
<xml_diff>
--- a/_LAYOUT.xlsx
+++ b/_LAYOUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\BinSortSequence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD963D67-659A-492D-9139-3938F5E85F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6B1B08-84EF-4D94-A6BB-2BAE379DDE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4517" uniqueCount="4410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4858" uniqueCount="4750">
   <si>
     <t>01-001-1</t>
   </si>
@@ -13265,6 +13265,1026 @@
   </si>
   <si>
     <t>9010-010</t>
+  </si>
+  <si>
+    <t>08-103-1</t>
+  </si>
+  <si>
+    <t>08-104-1</t>
+  </si>
+  <si>
+    <t>08-105-1</t>
+  </si>
+  <si>
+    <t>08-106-1</t>
+  </si>
+  <si>
+    <t>08-107-1</t>
+  </si>
+  <si>
+    <t>08-108-1</t>
+  </si>
+  <si>
+    <t>08-109-1</t>
+  </si>
+  <si>
+    <t>08-110-1</t>
+  </si>
+  <si>
+    <t>08-111-1</t>
+  </si>
+  <si>
+    <t>08-112-1</t>
+  </si>
+  <si>
+    <t>08-113-1</t>
+  </si>
+  <si>
+    <t>08-114-1</t>
+  </si>
+  <si>
+    <t>09-103-1</t>
+  </si>
+  <si>
+    <t>09-104-1</t>
+  </si>
+  <si>
+    <t>10-103-1</t>
+  </si>
+  <si>
+    <t>10-104-1</t>
+  </si>
+  <si>
+    <t>11-103-1</t>
+  </si>
+  <si>
+    <t>11-104-1</t>
+  </si>
+  <si>
+    <t>12-103-1</t>
+  </si>
+  <si>
+    <t>12-104-1</t>
+  </si>
+  <si>
+    <t>13-103-1</t>
+  </si>
+  <si>
+    <t>13-104-1</t>
+  </si>
+  <si>
+    <t>14-103-1</t>
+  </si>
+  <si>
+    <t>14-104-1</t>
+  </si>
+  <si>
+    <t>15-103-1</t>
+  </si>
+  <si>
+    <t>15-104-1</t>
+  </si>
+  <si>
+    <t>16-103-1</t>
+  </si>
+  <si>
+    <t>16-104-1</t>
+  </si>
+  <si>
+    <t>17-103-1</t>
+  </si>
+  <si>
+    <t>17-104-1</t>
+  </si>
+  <si>
+    <t>09-105-1</t>
+  </si>
+  <si>
+    <t>09-106-1</t>
+  </si>
+  <si>
+    <t>10-105-1</t>
+  </si>
+  <si>
+    <t>10-106-1</t>
+  </si>
+  <si>
+    <t>11-105-1</t>
+  </si>
+  <si>
+    <t>11-106-1</t>
+  </si>
+  <si>
+    <t>12-105-1</t>
+  </si>
+  <si>
+    <t>12-106-1</t>
+  </si>
+  <si>
+    <t>13-105-1</t>
+  </si>
+  <si>
+    <t>13-106-1</t>
+  </si>
+  <si>
+    <t>14-105-1</t>
+  </si>
+  <si>
+    <t>14-106-1</t>
+  </si>
+  <si>
+    <t>15-105-1</t>
+  </si>
+  <si>
+    <t>15-106-1</t>
+  </si>
+  <si>
+    <t>16-105-1</t>
+  </si>
+  <si>
+    <t>16-106-1</t>
+  </si>
+  <si>
+    <t>17-105-1</t>
+  </si>
+  <si>
+    <t>17-106-1</t>
+  </si>
+  <si>
+    <t>09-107-1</t>
+  </si>
+  <si>
+    <t>09-108-1</t>
+  </si>
+  <si>
+    <t>10-107-1</t>
+  </si>
+  <si>
+    <t>10-108-1</t>
+  </si>
+  <si>
+    <t>11-107-1</t>
+  </si>
+  <si>
+    <t>11-108-1</t>
+  </si>
+  <si>
+    <t>12-107-1</t>
+  </si>
+  <si>
+    <t>12-108-1</t>
+  </si>
+  <si>
+    <t>13-107-1</t>
+  </si>
+  <si>
+    <t>13-108-1</t>
+  </si>
+  <si>
+    <t>14-107-1</t>
+  </si>
+  <si>
+    <t>14-108-1</t>
+  </si>
+  <si>
+    <t>15-107-1</t>
+  </si>
+  <si>
+    <t>15-108-1</t>
+  </si>
+  <si>
+    <t>16-107-1</t>
+  </si>
+  <si>
+    <t>16-108-1</t>
+  </si>
+  <si>
+    <t>17-107-1</t>
+  </si>
+  <si>
+    <t>17-108-1</t>
+  </si>
+  <si>
+    <t>09-109-1</t>
+  </si>
+  <si>
+    <t>09-110-1</t>
+  </si>
+  <si>
+    <t>10-109-1</t>
+  </si>
+  <si>
+    <t>10-110-1</t>
+  </si>
+  <si>
+    <t>11-109-1</t>
+  </si>
+  <si>
+    <t>11-110-1</t>
+  </si>
+  <si>
+    <t>12-109-1</t>
+  </si>
+  <si>
+    <t>12-110-1</t>
+  </si>
+  <si>
+    <t>13-109-1</t>
+  </si>
+  <si>
+    <t>13-110-1</t>
+  </si>
+  <si>
+    <t>14-109-1</t>
+  </si>
+  <si>
+    <t>14-110-1</t>
+  </si>
+  <si>
+    <t>15-109-1</t>
+  </si>
+  <si>
+    <t>15-110-1</t>
+  </si>
+  <si>
+    <t>16-109-1</t>
+  </si>
+  <si>
+    <t>16-110-1</t>
+  </si>
+  <si>
+    <t>17-109-1</t>
+  </si>
+  <si>
+    <t>17-110-1</t>
+  </si>
+  <si>
+    <t>09-111-1</t>
+  </si>
+  <si>
+    <t>09-112-1</t>
+  </si>
+  <si>
+    <t>10-111-1</t>
+  </si>
+  <si>
+    <t>10-112-1</t>
+  </si>
+  <si>
+    <t>11-111-1</t>
+  </si>
+  <si>
+    <t>11-112-1</t>
+  </si>
+  <si>
+    <t>12-111-1</t>
+  </si>
+  <si>
+    <t>12-112-1</t>
+  </si>
+  <si>
+    <t>13-111-1</t>
+  </si>
+  <si>
+    <t>13-112-1</t>
+  </si>
+  <si>
+    <t>14-111-1</t>
+  </si>
+  <si>
+    <t>14-112-1</t>
+  </si>
+  <si>
+    <t>15-111-1</t>
+  </si>
+  <si>
+    <t>15-112-1</t>
+  </si>
+  <si>
+    <t>16-111-1</t>
+  </si>
+  <si>
+    <t>16-112-1</t>
+  </si>
+  <si>
+    <t>17-111-1</t>
+  </si>
+  <si>
+    <t>17-112-1</t>
+  </si>
+  <si>
+    <t>09-113-1</t>
+  </si>
+  <si>
+    <t>09-114-1</t>
+  </si>
+  <si>
+    <t>10-113-1</t>
+  </si>
+  <si>
+    <t>10-114-1</t>
+  </si>
+  <si>
+    <t>11-113-1</t>
+  </si>
+  <si>
+    <t>11-114-1</t>
+  </si>
+  <si>
+    <t>12-113-1</t>
+  </si>
+  <si>
+    <t>12-114-1</t>
+  </si>
+  <si>
+    <t>13-113-1</t>
+  </si>
+  <si>
+    <t>13-114-1</t>
+  </si>
+  <si>
+    <t>14-113-1</t>
+  </si>
+  <si>
+    <t>14-114-1</t>
+  </si>
+  <si>
+    <t>15-113-1</t>
+  </si>
+  <si>
+    <t>15-114-1</t>
+  </si>
+  <si>
+    <t>16-113-1</t>
+  </si>
+  <si>
+    <t>16-114-1</t>
+  </si>
+  <si>
+    <t>17-113-1</t>
+  </si>
+  <si>
+    <t>17-114-1</t>
+  </si>
+  <si>
+    <t>18-157-1</t>
+  </si>
+  <si>
+    <t>18-158-1</t>
+  </si>
+  <si>
+    <t>18-159-1</t>
+  </si>
+  <si>
+    <t>18-160-1</t>
+  </si>
+  <si>
+    <t>18-161-1</t>
+  </si>
+  <si>
+    <t>18-162-1</t>
+  </si>
+  <si>
+    <t>18-163-1</t>
+  </si>
+  <si>
+    <t>18-164-1</t>
+  </si>
+  <si>
+    <t>18-165-1</t>
+  </si>
+  <si>
+    <t>18-166-1</t>
+  </si>
+  <si>
+    <t>18-167-1</t>
+  </si>
+  <si>
+    <t>18-168-1</t>
+  </si>
+  <si>
+    <t>18-169-1</t>
+  </si>
+  <si>
+    <t>18-170-1</t>
+  </si>
+  <si>
+    <t>18-171-1</t>
+  </si>
+  <si>
+    <t>18-172-1</t>
+  </si>
+  <si>
+    <t>18-173-1</t>
+  </si>
+  <si>
+    <t>18-174-1</t>
+  </si>
+  <si>
+    <t>18-175-1</t>
+  </si>
+  <si>
+    <t>18-176-1</t>
+  </si>
+  <si>
+    <t>18-177-1</t>
+  </si>
+  <si>
+    <t>18-178-1</t>
+  </si>
+  <si>
+    <t>18-179-1</t>
+  </si>
+  <si>
+    <t>18-180-1</t>
+  </si>
+  <si>
+    <t>18-181-1</t>
+  </si>
+  <si>
+    <t>18-182-1</t>
+  </si>
+  <si>
+    <t>18-183-1</t>
+  </si>
+  <si>
+    <t>18-184-1</t>
+  </si>
+  <si>
+    <t>18-185-1</t>
+  </si>
+  <si>
+    <t>18-186-1</t>
+  </si>
+  <si>
+    <t>18-187-1</t>
+  </si>
+  <si>
+    <t>18-188-1</t>
+  </si>
+  <si>
+    <t>18-189-1</t>
+  </si>
+  <si>
+    <t>18-190-1</t>
+  </si>
+  <si>
+    <t>18-191-1</t>
+  </si>
+  <si>
+    <t>18-192-1</t>
+  </si>
+  <si>
+    <t>18-193-1</t>
+  </si>
+  <si>
+    <t>18-194-1</t>
+  </si>
+  <si>
+    <t>18-195-1</t>
+  </si>
+  <si>
+    <t>18-196-1</t>
+  </si>
+  <si>
+    <t>18-197-1</t>
+  </si>
+  <si>
+    <t>18-198-1</t>
+  </si>
+  <si>
+    <t>18-199-1</t>
+  </si>
+  <si>
+    <t>18-200-1</t>
+  </si>
+  <si>
+    <t>18-201-1</t>
+  </si>
+  <si>
+    <t>18-202-1</t>
+  </si>
+  <si>
+    <t>18-203-1</t>
+  </si>
+  <si>
+    <t>18-204-1</t>
+  </si>
+  <si>
+    <t>18-205-1</t>
+  </si>
+  <si>
+    <t>18-206-1</t>
+  </si>
+  <si>
+    <t>18-207-1</t>
+  </si>
+  <si>
+    <t>18-208-1</t>
+  </si>
+  <si>
+    <t>18-209-1</t>
+  </si>
+  <si>
+    <t>18-210-1</t>
+  </si>
+  <si>
+    <t>18-211-1</t>
+  </si>
+  <si>
+    <t>18-212-1</t>
+  </si>
+  <si>
+    <t>18-213-1</t>
+  </si>
+  <si>
+    <t>18-214-1</t>
+  </si>
+  <si>
+    <t>18-215-1</t>
+  </si>
+  <si>
+    <t>18-216-1</t>
+  </si>
+  <si>
+    <t>18-217-1</t>
+  </si>
+  <si>
+    <t>18-218-1</t>
+  </si>
+  <si>
+    <t>18-219-1</t>
+  </si>
+  <si>
+    <t>18-220-1</t>
+  </si>
+  <si>
+    <t>18-221-1</t>
+  </si>
+  <si>
+    <t>18-222-1</t>
+  </si>
+  <si>
+    <t>18-223-1</t>
+  </si>
+  <si>
+    <t>18-224-1</t>
+  </si>
+  <si>
+    <t>18-225-1</t>
+  </si>
+  <si>
+    <t>18-226-1</t>
+  </si>
+  <si>
+    <t>18-227-1</t>
+  </si>
+  <si>
+    <t>18-228-1</t>
+  </si>
+  <si>
+    <t>18-229-1</t>
+  </si>
+  <si>
+    <t>18-230-1</t>
+  </si>
+  <si>
+    <t>18-231-1</t>
+  </si>
+  <si>
+    <t>18-232-1</t>
+  </si>
+  <si>
+    <t>18-233-1</t>
+  </si>
+  <si>
+    <t>18-234-1</t>
+  </si>
+  <si>
+    <t>18-235-1</t>
+  </si>
+  <si>
+    <t>18-236-1</t>
+  </si>
+  <si>
+    <t>18-237-1</t>
+  </si>
+  <si>
+    <t>18-238-1</t>
+  </si>
+  <si>
+    <t>18-239-1</t>
+  </si>
+  <si>
+    <t>18-240-1</t>
+  </si>
+  <si>
+    <t>18-241-1</t>
+  </si>
+  <si>
+    <t>18-242-1</t>
+  </si>
+  <si>
+    <t>18-243-1</t>
+  </si>
+  <si>
+    <t>18-244-1</t>
+  </si>
+  <si>
+    <t>18-245-1</t>
+  </si>
+  <si>
+    <t>18-246-1</t>
+  </si>
+  <si>
+    <t>18-247-1</t>
+  </si>
+  <si>
+    <t>18-248-1</t>
+  </si>
+  <si>
+    <t>18-249-1</t>
+  </si>
+  <si>
+    <t>18-250-1</t>
+  </si>
+  <si>
+    <t>18-251-1</t>
+  </si>
+  <si>
+    <t>18-252-1</t>
+  </si>
+  <si>
+    <t>9010-011</t>
+  </si>
+  <si>
+    <t>9010-012</t>
+  </si>
+  <si>
+    <t>9010-013</t>
+  </si>
+  <si>
+    <t>9010-014</t>
+  </si>
+  <si>
+    <t>9010-015</t>
+  </si>
+  <si>
+    <t>9010-016</t>
+  </si>
+  <si>
+    <t>9010-017</t>
+  </si>
+  <si>
+    <t>9010-018</t>
+  </si>
+  <si>
+    <t>9010-019</t>
+  </si>
+  <si>
+    <t>9010-020</t>
+  </si>
+  <si>
+    <t>9010-021</t>
+  </si>
+  <si>
+    <t>9010-022</t>
+  </si>
+  <si>
+    <t>9010-023</t>
+  </si>
+  <si>
+    <t>9010-024</t>
+  </si>
+  <si>
+    <t>9010-025</t>
+  </si>
+  <si>
+    <t>9010-026</t>
+  </si>
+  <si>
+    <t>9010-027</t>
+  </si>
+  <si>
+    <t>9010-028</t>
+  </si>
+  <si>
+    <t>9010-029</t>
+  </si>
+  <si>
+    <t>9010-030</t>
+  </si>
+  <si>
+    <t>9010-031</t>
+  </si>
+  <si>
+    <t>9010-032</t>
+  </si>
+  <si>
+    <t>9010-033</t>
+  </si>
+  <si>
+    <t>9010-034</t>
+  </si>
+  <si>
+    <t>9010-035</t>
+  </si>
+  <si>
+    <t>9010-036</t>
+  </si>
+  <si>
+    <t>9010-037</t>
+  </si>
+  <si>
+    <t>9020-011</t>
+  </si>
+  <si>
+    <t>9020-012</t>
+  </si>
+  <si>
+    <t>9020-013</t>
+  </si>
+  <si>
+    <t>9020-014</t>
+  </si>
+  <si>
+    <t>9020-015</t>
+  </si>
+  <si>
+    <t>9020-016</t>
+  </si>
+  <si>
+    <t>9020-017</t>
+  </si>
+  <si>
+    <t>9020-018</t>
+  </si>
+  <si>
+    <t>9020-019</t>
+  </si>
+  <si>
+    <t>9020-020</t>
+  </si>
+  <si>
+    <t>9020-021</t>
+  </si>
+  <si>
+    <t>9020-022</t>
+  </si>
+  <si>
+    <t>9020-023</t>
+  </si>
+  <si>
+    <t>9020-024</t>
+  </si>
+  <si>
+    <t>9020-025</t>
+  </si>
+  <si>
+    <t>9020-026</t>
+  </si>
+  <si>
+    <t>9020-027</t>
+  </si>
+  <si>
+    <t>9020-028</t>
+  </si>
+  <si>
+    <t>9020-029</t>
+  </si>
+  <si>
+    <t>9020-030</t>
+  </si>
+  <si>
+    <t>9020-031</t>
+  </si>
+  <si>
+    <t>9020-032</t>
+  </si>
+  <si>
+    <t>9020-033</t>
+  </si>
+  <si>
+    <t>9020-034</t>
+  </si>
+  <si>
+    <t>9020-035</t>
+  </si>
+  <si>
+    <t>9020-036</t>
+  </si>
+  <si>
+    <t>9020-037</t>
+  </si>
+  <si>
+    <t>9020-038</t>
+  </si>
+  <si>
+    <t>9020-039</t>
+  </si>
+  <si>
+    <t>9020-040</t>
+  </si>
+  <si>
+    <t>9020-041</t>
+  </si>
+  <si>
+    <t>9020-042</t>
+  </si>
+  <si>
+    <t>9020-043</t>
+  </si>
+  <si>
+    <t>9020-044</t>
+  </si>
+  <si>
+    <t>9020-045</t>
+  </si>
+  <si>
+    <t>9020-046</t>
+  </si>
+  <si>
+    <t>9020-047</t>
+  </si>
+  <si>
+    <t>9020-048</t>
+  </si>
+  <si>
+    <t>9020-049</t>
+  </si>
+  <si>
+    <t>9020-050</t>
+  </si>
+  <si>
+    <t>9020-051</t>
+  </si>
+  <si>
+    <t>9020-052</t>
+  </si>
+  <si>
+    <t>9020-053</t>
+  </si>
+  <si>
+    <t>9020-054</t>
+  </si>
+  <si>
+    <t>9020-055</t>
+  </si>
+  <si>
+    <t>9020-056</t>
+  </si>
+  <si>
+    <t>9020-057</t>
+  </si>
+  <si>
+    <t>9020-058</t>
+  </si>
+  <si>
+    <t>9020-059</t>
+  </si>
+  <si>
+    <t>9020-060</t>
+  </si>
+  <si>
+    <t>9020-061</t>
+  </si>
+  <si>
+    <t>9020-062</t>
+  </si>
+  <si>
+    <t>9020-063</t>
+  </si>
+  <si>
+    <t>9020-064</t>
+  </si>
+  <si>
+    <t>9020-065</t>
+  </si>
+  <si>
+    <t>9020-066</t>
+  </si>
+  <si>
+    <t>9020-067</t>
+  </si>
+  <si>
+    <t>9020-068</t>
+  </si>
+  <si>
+    <t>9020-069</t>
+  </si>
+  <si>
+    <t>9020-070</t>
+  </si>
+  <si>
+    <t>9020-071</t>
+  </si>
+  <si>
+    <t>9020-072</t>
+  </si>
+  <si>
+    <t>9020-073</t>
+  </si>
+  <si>
+    <t>9020-074</t>
+  </si>
+  <si>
+    <t>9020-075</t>
+  </si>
+  <si>
+    <t>9020-076</t>
+  </si>
+  <si>
+    <t>9020-077</t>
+  </si>
+  <si>
+    <t>9020-078</t>
+  </si>
+  <si>
+    <t>9020-079</t>
+  </si>
+  <si>
+    <t>9020-080</t>
+  </si>
+  <si>
+    <t>9020-081</t>
+  </si>
+  <si>
+    <t>9020-082</t>
+  </si>
+  <si>
+    <t>9020-083</t>
+  </si>
+  <si>
+    <t>9020-084</t>
+  </si>
+  <si>
+    <t>9020-085</t>
+  </si>
+  <si>
+    <t>9020-086</t>
+  </si>
+  <si>
+    <t>9020-087</t>
+  </si>
+  <si>
+    <t>9020-088</t>
+  </si>
+  <si>
+    <t>9020-089</t>
+  </si>
+  <si>
+    <t>9020-090</t>
+  </si>
+  <si>
+    <t>9020-091</t>
+  </si>
+  <si>
+    <t>9020-092</t>
+  </si>
+  <si>
+    <t>9020-093</t>
+  </si>
+  <si>
+    <t>9020-094</t>
+  </si>
+  <si>
+    <t>9020-095</t>
+  </si>
+  <si>
+    <t>9020-096</t>
+  </si>
+  <si>
+    <t>9020-097</t>
+  </si>
+  <si>
+    <t>9020-098</t>
+  </si>
+  <si>
+    <t>9020-099</t>
+  </si>
+  <si>
+    <t>9020-100</t>
+  </si>
+  <si>
+    <t>9020-101</t>
+  </si>
+  <si>
+    <t>0103-001</t>
+  </si>
+  <si>
+    <t>0108-001</t>
+  </si>
+  <si>
+    <t>0109-001</t>
+  </si>
+  <si>
+    <t>8040-001</t>
+  </si>
+  <si>
+    <t>8040-002</t>
+  </si>
+  <si>
+    <t>8040-003</t>
   </si>
 </sst>
 </file>
@@ -13754,10 +14774,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -14134,10 +15157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF127"/>
+  <dimension ref="A1:BG127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BC7" sqref="BC7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14171,11 +15194,11 @@
     <col min="50" max="51" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="53" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="54" max="55" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="16384" width="9.140625" style="1"/>
+    <col min="56" max="59" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2821</v>
       </c>
@@ -14350,8 +15373,11 @@
       <c r="BF1" s="1" t="s">
         <v>4379</v>
       </c>
+      <c r="BG1" s="1" t="s">
+        <v>4379</v>
+      </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -14520,14 +15546,17 @@
       <c r="BD2" s="1" t="s">
         <v>4390</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BE2" s="2" t="s">
         <v>4400</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BF2" s="2" t="s">
         <v>4380</v>
       </c>
+      <c r="BG2" s="2" t="s">
+        <v>4744</v>
+      </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -14696,14 +15725,17 @@
       <c r="BD3" s="1" t="s">
         <v>4391</v>
       </c>
-      <c r="BE3" s="1" t="s">
+      <c r="BE3" s="2" t="s">
         <v>4401</v>
       </c>
-      <c r="BF3" s="1" t="s">
+      <c r="BF3" s="2" t="s">
         <v>4385</v>
       </c>
+      <c r="BG3" s="2" t="s">
+        <v>4745</v>
+      </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>110</v>
       </c>
@@ -14872,14 +15904,17 @@
       <c r="BD4" s="1" t="s">
         <v>4392</v>
       </c>
-      <c r="BE4" s="1" t="s">
+      <c r="BE4" s="2" t="s">
         <v>4402</v>
       </c>
-      <c r="BF4" s="1" t="s">
+      <c r="BF4" s="2" t="s">
         <v>4381</v>
       </c>
+      <c r="BG4" s="2" t="s">
+        <v>4746</v>
+      </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>165</v>
       </c>
@@ -15048,14 +16083,17 @@
       <c r="BD5" s="1" t="s">
         <v>4393</v>
       </c>
-      <c r="BE5" s="1" t="s">
+      <c r="BE5" s="2" t="s">
         <v>4403</v>
       </c>
-      <c r="BF5" s="1" t="s">
+      <c r="BF5" s="2" t="s">
         <v>4386</v>
       </c>
+      <c r="BG5" s="2" t="s">
+        <v>4747</v>
+      </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>220</v>
       </c>
@@ -15224,14 +16262,17 @@
       <c r="BD6" s="1" t="s">
         <v>4394</v>
       </c>
-      <c r="BE6" s="1" t="s">
+      <c r="BE6" s="2" t="s">
         <v>4404</v>
       </c>
-      <c r="BF6" s="1" t="s">
+      <c r="BF6" s="2" t="s">
         <v>4382</v>
       </c>
+      <c r="BG6" s="2" t="s">
+        <v>4748</v>
+      </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>275</v>
       </c>
@@ -15400,14 +16441,17 @@
       <c r="BD7" s="1" t="s">
         <v>4395</v>
       </c>
-      <c r="BE7" s="1" t="s">
+      <c r="BE7" s="2" t="s">
         <v>4405</v>
       </c>
-      <c r="BF7" s="1" t="s">
+      <c r="BF7" s="2" t="s">
         <v>4387</v>
       </c>
+      <c r="BG7" s="2" t="s">
+        <v>4749</v>
+      </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>330</v>
       </c>
@@ -15576,14 +16620,14 @@
       <c r="BD8" s="1" t="s">
         <v>4396</v>
       </c>
-      <c r="BE8" s="1" t="s">
+      <c r="BE8" s="2" t="s">
         <v>4406</v>
       </c>
-      <c r="BF8" s="1" t="s">
+      <c r="BF8" s="2" t="s">
         <v>4383</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>385</v>
       </c>
@@ -15752,14 +16796,14 @@
       <c r="BD9" s="1" t="s">
         <v>4397</v>
       </c>
-      <c r="BE9" s="1" t="s">
+      <c r="BE9" s="2" t="s">
         <v>4407</v>
       </c>
-      <c r="BF9" s="1" t="s">
+      <c r="BF9" s="2" t="s">
         <v>4388</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>440</v>
       </c>
@@ -15928,14 +16972,14 @@
       <c r="BD10" s="1" t="s">
         <v>4398</v>
       </c>
-      <c r="BE10" s="1" t="s">
+      <c r="BE10" s="2" t="s">
         <v>4408</v>
       </c>
-      <c r="BF10" s="1" t="s">
+      <c r="BF10" s="2" t="s">
         <v>4384</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>495</v>
       </c>
@@ -16104,14 +17148,14 @@
       <c r="BD11" s="1" t="s">
         <v>4399</v>
       </c>
-      <c r="BE11" s="1" t="s">
+      <c r="BE11" s="2" t="s">
         <v>4409</v>
       </c>
-      <c r="BF11" s="1" t="s">
+      <c r="BF11" s="2" t="s">
         <v>4389</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>550</v>
       </c>
@@ -16277,8 +17321,14 @@
       <c r="BC12" s="1" t="s">
         <v>604</v>
       </c>
+      <c r="BE12" s="2" t="s">
+        <v>4626</v>
+      </c>
+      <c r="BF12" s="2" t="s">
+        <v>4653</v>
+      </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>605</v>
       </c>
@@ -16444,8 +17494,14 @@
       <c r="BC13" s="1" t="s">
         <v>659</v>
       </c>
+      <c r="BE13" s="2" t="s">
+        <v>4627</v>
+      </c>
+      <c r="BF13" s="2" t="s">
+        <v>4654</v>
+      </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>660</v>
       </c>
@@ -16611,8 +17667,14 @@
       <c r="BC14" s="1" t="s">
         <v>714</v>
       </c>
+      <c r="BE14" s="2" t="s">
+        <v>4628</v>
+      </c>
+      <c r="BF14" s="2" t="s">
+        <v>4655</v>
+      </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>715</v>
       </c>
@@ -16778,8 +17840,14 @@
       <c r="BC15" s="1" t="s">
         <v>769</v>
       </c>
+      <c r="BE15" s="2" t="s">
+        <v>4629</v>
+      </c>
+      <c r="BF15" s="2" t="s">
+        <v>4656</v>
+      </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>770</v>
       </c>
@@ -16945,8 +18013,14 @@
       <c r="BC16" s="1" t="s">
         <v>824</v>
       </c>
+      <c r="BE16" s="2" t="s">
+        <v>4630</v>
+      </c>
+      <c r="BF16" s="2" t="s">
+        <v>4657</v>
+      </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>825</v>
       </c>
@@ -17112,8 +18186,14 @@
       <c r="BC17" s="1" t="s">
         <v>879</v>
       </c>
+      <c r="BE17" s="2" t="s">
+        <v>4631</v>
+      </c>
+      <c r="BF17" s="2" t="s">
+        <v>4658</v>
+      </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>880</v>
       </c>
@@ -17279,8 +18359,14 @@
       <c r="BC18" s="1" t="s">
         <v>934</v>
       </c>
+      <c r="BE18" s="2" t="s">
+        <v>4632</v>
+      </c>
+      <c r="BF18" s="2" t="s">
+        <v>4659</v>
+      </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>935</v>
       </c>
@@ -17446,8 +18532,14 @@
       <c r="BC19" s="1" t="s">
         <v>989</v>
       </c>
+      <c r="BE19" s="2" t="s">
+        <v>4633</v>
+      </c>
+      <c r="BF19" s="2" t="s">
+        <v>4660</v>
+      </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>990</v>
       </c>
@@ -17613,8 +18705,14 @@
       <c r="BC20" s="1" t="s">
         <v>1044</v>
       </c>
+      <c r="BE20" s="2" t="s">
+        <v>4634</v>
+      </c>
+      <c r="BF20" s="2" t="s">
+        <v>4661</v>
+      </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1045</v>
       </c>
@@ -17780,8 +18878,14 @@
       <c r="BC21" s="1" t="s">
         <v>1099</v>
       </c>
+      <c r="BE21" s="2" t="s">
+        <v>4635</v>
+      </c>
+      <c r="BF21" s="2" t="s">
+        <v>4662</v>
+      </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>1100</v>
       </c>
@@ -17947,8 +19051,14 @@
       <c r="BC22" s="1" t="s">
         <v>1154</v>
       </c>
+      <c r="BE22" s="2" t="s">
+        <v>4636</v>
+      </c>
+      <c r="BF22" s="2" t="s">
+        <v>4663</v>
+      </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1155</v>
       </c>
@@ -18114,8 +19224,14 @@
       <c r="BC23" s="1" t="s">
         <v>1209</v>
       </c>
+      <c r="BE23" s="2" t="s">
+        <v>4637</v>
+      </c>
+      <c r="BF23" s="2" t="s">
+        <v>4664</v>
+      </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1210</v>
       </c>
@@ -18281,8 +19397,14 @@
       <c r="BC24" s="1" t="s">
         <v>1264</v>
       </c>
+      <c r="BE24" s="2" t="s">
+        <v>4638</v>
+      </c>
+      <c r="BF24" s="2" t="s">
+        <v>4665</v>
+      </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1265</v>
       </c>
@@ -18448,8 +19570,14 @@
       <c r="BC25" s="1" t="s">
         <v>1319</v>
       </c>
+      <c r="BE25" s="2" t="s">
+        <v>4639</v>
+      </c>
+      <c r="BF25" s="2" t="s">
+        <v>4666</v>
+      </c>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>1320</v>
       </c>
@@ -18615,8 +19743,14 @@
       <c r="BC26" s="1" t="s">
         <v>1374</v>
       </c>
+      <c r="BE26" s="2" t="s">
+        <v>4640</v>
+      </c>
+      <c r="BF26" s="2" t="s">
+        <v>4667</v>
+      </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1375</v>
       </c>
@@ -18782,8 +19916,14 @@
       <c r="BC27" s="1" t="s">
         <v>1429</v>
       </c>
+      <c r="BE27" s="2" t="s">
+        <v>4641</v>
+      </c>
+      <c r="BF27" s="2" t="s">
+        <v>4668</v>
+      </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>1430</v>
       </c>
@@ -18949,8 +20089,14 @@
       <c r="BC28" s="1" t="s">
         <v>1484</v>
       </c>
+      <c r="BE28" s="2" t="s">
+        <v>4642</v>
+      </c>
+      <c r="BF28" s="2" t="s">
+        <v>4669</v>
+      </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1485</v>
       </c>
@@ -19116,8 +20262,14 @@
       <c r="BC29" s="1" t="s">
         <v>1539</v>
       </c>
+      <c r="BE29" s="2" t="s">
+        <v>4643</v>
+      </c>
+      <c r="BF29" s="2" t="s">
+        <v>4670</v>
+      </c>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>1540</v>
       </c>
@@ -19283,8 +20435,14 @@
       <c r="BC30" s="1" t="s">
         <v>1594</v>
       </c>
+      <c r="BE30" s="2" t="s">
+        <v>4644</v>
+      </c>
+      <c r="BF30" s="2" t="s">
+        <v>4671</v>
+      </c>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>1595</v>
       </c>
@@ -19450,8 +20608,14 @@
       <c r="BC31" s="1" t="s">
         <v>1649</v>
       </c>
+      <c r="BE31" s="2" t="s">
+        <v>4645</v>
+      </c>
+      <c r="BF31" s="2" t="s">
+        <v>4672</v>
+      </c>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>1650</v>
       </c>
@@ -19617,8 +20781,14 @@
       <c r="BC32" s="1" t="s">
         <v>1704</v>
       </c>
+      <c r="BE32" s="2" t="s">
+        <v>4646</v>
+      </c>
+      <c r="BF32" s="2" t="s">
+        <v>4673</v>
+      </c>
     </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>1705</v>
       </c>
@@ -19784,8 +20954,14 @@
       <c r="BC33" s="1" t="s">
         <v>1759</v>
       </c>
+      <c r="BE33" s="2" t="s">
+        <v>4647</v>
+      </c>
+      <c r="BF33" s="2" t="s">
+        <v>4674</v>
+      </c>
     </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1760</v>
       </c>
@@ -19951,8 +21127,14 @@
       <c r="BC34" s="1" t="s">
         <v>1814</v>
       </c>
+      <c r="BE34" s="2" t="s">
+        <v>4648</v>
+      </c>
+      <c r="BF34" s="2" t="s">
+        <v>4675</v>
+      </c>
     </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1815</v>
       </c>
@@ -20118,8 +21300,14 @@
       <c r="BC35" s="1" t="s">
         <v>1869</v>
       </c>
+      <c r="BE35" s="2" t="s">
+        <v>4649</v>
+      </c>
+      <c r="BF35" s="2" t="s">
+        <v>4676</v>
+      </c>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1870</v>
       </c>
@@ -20285,8 +21473,14 @@
       <c r="BC36" s="1" t="s">
         <v>1924</v>
       </c>
+      <c r="BE36" s="2" t="s">
+        <v>4650</v>
+      </c>
+      <c r="BF36" s="2" t="s">
+        <v>4677</v>
+      </c>
     </row>
-    <row r="37" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>1925</v>
       </c>
@@ -20452,8 +21646,14 @@
       <c r="BC37" s="1" t="s">
         <v>1979</v>
       </c>
+      <c r="BE37" s="2" t="s">
+        <v>4651</v>
+      </c>
+      <c r="BF37" s="2" t="s">
+        <v>4678</v>
+      </c>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>1980</v>
       </c>
@@ -20619,8 +21819,14 @@
       <c r="BC38" s="1" t="s">
         <v>2034</v>
       </c>
+      <c r="BE38" s="2" t="s">
+        <v>4652</v>
+      </c>
+      <c r="BF38" s="2" t="s">
+        <v>4679</v>
+      </c>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>2035</v>
       </c>
@@ -20786,8 +21992,11 @@
       <c r="BC39" s="1" t="s">
         <v>2089</v>
       </c>
+      <c r="BF39" s="2" t="s">
+        <v>4680</v>
+      </c>
     </row>
-    <row r="40" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>2090</v>
       </c>
@@ -20953,8 +22162,11 @@
       <c r="BC40" s="1" t="s">
         <v>2144</v>
       </c>
+      <c r="BF40" s="2" t="s">
+        <v>4681</v>
+      </c>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>2145</v>
       </c>
@@ -21120,8 +22332,11 @@
       <c r="BC41" s="1" t="s">
         <v>2199</v>
       </c>
+      <c r="BF41" s="2" t="s">
+        <v>4682</v>
+      </c>
     </row>
-    <row r="42" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>2200</v>
       </c>
@@ -21287,8 +22502,11 @@
       <c r="BC42" s="1" t="s">
         <v>2254</v>
       </c>
+      <c r="BF42" s="2" t="s">
+        <v>4683</v>
+      </c>
     </row>
-    <row r="43" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>2255</v>
       </c>
@@ -21454,8 +22672,11 @@
       <c r="BC43" s="1" t="s">
         <v>2309</v>
       </c>
+      <c r="BF43" s="2" t="s">
+        <v>4684</v>
+      </c>
     </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>2310</v>
       </c>
@@ -21621,8 +22842,11 @@
       <c r="BC44" s="1" t="s">
         <v>2364</v>
       </c>
+      <c r="BF44" s="2" t="s">
+        <v>4685</v>
+      </c>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>2365</v>
       </c>
@@ -21788,8 +23012,11 @@
       <c r="BC45" s="1" t="s">
         <v>2419</v>
       </c>
+      <c r="BF45" s="2" t="s">
+        <v>4686</v>
+      </c>
     </row>
-    <row r="46" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>2420</v>
       </c>
@@ -21955,8 +23182,11 @@
       <c r="BC46" s="1" t="s">
         <v>2474</v>
       </c>
+      <c r="BF46" s="2" t="s">
+        <v>4687</v>
+      </c>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>2475</v>
       </c>
@@ -22122,8 +23352,11 @@
       <c r="BC47" s="1" t="s">
         <v>2529</v>
       </c>
+      <c r="BF47" s="2" t="s">
+        <v>4688</v>
+      </c>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>2530</v>
       </c>
@@ -22289,8 +23522,11 @@
       <c r="BC48" s="1" t="s">
         <v>2584</v>
       </c>
+      <c r="BF48" s="2" t="s">
+        <v>4689</v>
+      </c>
     </row>
-    <row r="49" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>2585</v>
       </c>
@@ -22456,8 +23692,11 @@
       <c r="BC49" s="1" t="s">
         <v>2639</v>
       </c>
+      <c r="BF49" s="2" t="s">
+        <v>4690</v>
+      </c>
     </row>
-    <row r="50" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>2640</v>
       </c>
@@ -22623,8 +23862,11 @@
       <c r="BC50" s="1" t="s">
         <v>2694</v>
       </c>
+      <c r="BF50" s="2" t="s">
+        <v>4691</v>
+      </c>
     </row>
-    <row r="51" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>2695</v>
       </c>
@@ -22790,8 +24032,11 @@
       <c r="BC51" s="1" t="s">
         <v>2749</v>
       </c>
+      <c r="BF51" s="2" t="s">
+        <v>4692</v>
+      </c>
     </row>
-    <row r="52" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>2750</v>
       </c>
@@ -22957,10 +24202,76 @@
       <c r="BC52" s="1" t="s">
         <v>2804</v>
       </c>
+      <c r="BF52" s="2" t="s">
+        <v>4693</v>
+      </c>
     </row>
-    <row r="53" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI53" s="1" t="s">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N53" s="2" t="s">
+        <v>4410</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>4411</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>4422</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>4423</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>4424</v>
+      </c>
+      <c r="S53" s="2" t="s">
+        <v>4425</v>
+      </c>
+      <c r="T53" s="2" t="s">
+        <v>4426</v>
+      </c>
+      <c r="U53" s="2" t="s">
+        <v>4427</v>
+      </c>
+      <c r="V53" s="2" t="s">
+        <v>4428</v>
+      </c>
+      <c r="W53" s="2" t="s">
+        <v>4429</v>
+      </c>
+      <c r="X53" s="2" t="s">
+        <v>4430</v>
+      </c>
+      <c r="Y53" s="2" t="s">
+        <v>4431</v>
+      </c>
+      <c r="Z53" s="2" t="s">
+        <v>4432</v>
+      </c>
+      <c r="AA53" s="2" t="s">
+        <v>4433</v>
+      </c>
+      <c r="AB53" s="2" t="s">
+        <v>4434</v>
+      </c>
+      <c r="AC53" s="2" t="s">
+        <v>4435</v>
+      </c>
+      <c r="AD53" s="2" t="s">
+        <v>4436</v>
+      </c>
+      <c r="AE53" s="2" t="s">
+        <v>4437</v>
+      </c>
+      <c r="AF53" s="2" t="s">
+        <v>4438</v>
+      </c>
+      <c r="AG53" s="2" t="s">
+        <v>4439</v>
+      </c>
+      <c r="AH53" s="2" t="s">
         <v>2825</v>
+      </c>
+      <c r="AI53" s="2" t="s">
+        <v>2826</v>
       </c>
       <c r="AJ53" s="1" t="s">
         <v>2879</v>
@@ -23022,10 +24333,76 @@
       <c r="BC53" s="1" t="s">
         <v>3046</v>
       </c>
+      <c r="BF53" s="2" t="s">
+        <v>4694</v>
+      </c>
     </row>
-    <row r="54" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI54" s="1" t="s">
-        <v>2826</v>
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N54" s="2" t="s">
+        <v>4412</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>4413</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>4440</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>4441</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>4442</v>
+      </c>
+      <c r="S54" s="2" t="s">
+        <v>4443</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>4444</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>4445</v>
+      </c>
+      <c r="V54" s="2" t="s">
+        <v>4446</v>
+      </c>
+      <c r="W54" s="2" t="s">
+        <v>4447</v>
+      </c>
+      <c r="X54" s="2" t="s">
+        <v>4448</v>
+      </c>
+      <c r="Y54" s="2" t="s">
+        <v>4449</v>
+      </c>
+      <c r="Z54" s="2" t="s">
+        <v>4450</v>
+      </c>
+      <c r="AA54" s="2" t="s">
+        <v>4451</v>
+      </c>
+      <c r="AB54" s="2" t="s">
+        <v>4452</v>
+      </c>
+      <c r="AC54" s="2" t="s">
+        <v>4453</v>
+      </c>
+      <c r="AD54" s="2" t="s">
+        <v>4454</v>
+      </c>
+      <c r="AE54" s="2" t="s">
+        <v>4455</v>
+      </c>
+      <c r="AF54" s="2" t="s">
+        <v>4456</v>
+      </c>
+      <c r="AG54" s="2" t="s">
+        <v>4457</v>
+      </c>
+      <c r="AH54" s="2" t="s">
+        <v>2827</v>
+      </c>
+      <c r="AI54" s="2" t="s">
+        <v>2828</v>
       </c>
       <c r="AJ54" s="1" t="s">
         <v>2881</v>
@@ -23087,10 +24464,76 @@
       <c r="BC54" s="1" t="s">
         <v>3064</v>
       </c>
+      <c r="BF54" s="2" t="s">
+        <v>4695</v>
+      </c>
     </row>
-    <row r="55" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI55" s="1" t="s">
-        <v>2827</v>
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N55" s="2" t="s">
+        <v>4414</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>4415</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>4458</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>4459</v>
+      </c>
+      <c r="R55" s="2" t="s">
+        <v>4460</v>
+      </c>
+      <c r="S55" s="2" t="s">
+        <v>4461</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>4462</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>4463</v>
+      </c>
+      <c r="V55" s="2" t="s">
+        <v>4464</v>
+      </c>
+      <c r="W55" s="2" t="s">
+        <v>4465</v>
+      </c>
+      <c r="X55" s="2" t="s">
+        <v>4466</v>
+      </c>
+      <c r="Y55" s="2" t="s">
+        <v>4467</v>
+      </c>
+      <c r="Z55" s="2" t="s">
+        <v>4468</v>
+      </c>
+      <c r="AA55" s="2" t="s">
+        <v>4469</v>
+      </c>
+      <c r="AB55" s="2" t="s">
+        <v>4470</v>
+      </c>
+      <c r="AC55" s="2" t="s">
+        <v>4471</v>
+      </c>
+      <c r="AD55" s="2" t="s">
+        <v>4472</v>
+      </c>
+      <c r="AE55" s="2" t="s">
+        <v>4473</v>
+      </c>
+      <c r="AF55" s="2" t="s">
+        <v>4474</v>
+      </c>
+      <c r="AG55" s="2" t="s">
+        <v>4475</v>
+      </c>
+      <c r="AH55" s="2" t="s">
+        <v>2829</v>
+      </c>
+      <c r="AI55" s="2" t="s">
+        <v>2830</v>
       </c>
       <c r="AJ55" s="1" t="s">
         <v>2883</v>
@@ -23152,10 +24595,76 @@
       <c r="BC55" s="1" t="s">
         <v>3082</v>
       </c>
+      <c r="BF55" s="2" t="s">
+        <v>4696</v>
+      </c>
     </row>
-    <row r="56" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI56" s="1" t="s">
-        <v>2828</v>
+    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N56" s="2" t="s">
+        <v>4416</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>4417</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>4476</v>
+      </c>
+      <c r="Q56" s="2" t="s">
+        <v>4477</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>4478</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>4479</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>4480</v>
+      </c>
+      <c r="U56" s="2" t="s">
+        <v>4481</v>
+      </c>
+      <c r="V56" s="2" t="s">
+        <v>4482</v>
+      </c>
+      <c r="W56" s="2" t="s">
+        <v>4483</v>
+      </c>
+      <c r="X56" s="2" t="s">
+        <v>4484</v>
+      </c>
+      <c r="Y56" s="2" t="s">
+        <v>4485</v>
+      </c>
+      <c r="Z56" s="2" t="s">
+        <v>4486</v>
+      </c>
+      <c r="AA56" s="2" t="s">
+        <v>4487</v>
+      </c>
+      <c r="AB56" s="2" t="s">
+        <v>4488</v>
+      </c>
+      <c r="AC56" s="2" t="s">
+        <v>4489</v>
+      </c>
+      <c r="AD56" s="2" t="s">
+        <v>4490</v>
+      </c>
+      <c r="AE56" s="2" t="s">
+        <v>4491</v>
+      </c>
+      <c r="AF56" s="2" t="s">
+        <v>4492</v>
+      </c>
+      <c r="AG56" s="2" t="s">
+        <v>4493</v>
+      </c>
+      <c r="AH56" s="2" t="s">
+        <v>2831</v>
+      </c>
+      <c r="AI56" s="2" t="s">
+        <v>2832</v>
       </c>
       <c r="AJ56" s="1" t="s">
         <v>2885</v>
@@ -23217,10 +24726,76 @@
       <c r="BC56" s="1" t="s">
         <v>3100</v>
       </c>
+      <c r="BF56" s="2" t="s">
+        <v>4697</v>
+      </c>
     </row>
-    <row r="57" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI57" s="1" t="s">
-        <v>2829</v>
+    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N57" s="2" t="s">
+        <v>4418</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>4419</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>4494</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>4495</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>4496</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>4497</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>4498</v>
+      </c>
+      <c r="U57" s="2" t="s">
+        <v>4499</v>
+      </c>
+      <c r="V57" s="2" t="s">
+        <v>4500</v>
+      </c>
+      <c r="W57" s="2" t="s">
+        <v>4501</v>
+      </c>
+      <c r="X57" s="2" t="s">
+        <v>4502</v>
+      </c>
+      <c r="Y57" s="2" t="s">
+        <v>4503</v>
+      </c>
+      <c r="Z57" s="2" t="s">
+        <v>4504</v>
+      </c>
+      <c r="AA57" s="2" t="s">
+        <v>4505</v>
+      </c>
+      <c r="AB57" s="2" t="s">
+        <v>4506</v>
+      </c>
+      <c r="AC57" s="2" t="s">
+        <v>4507</v>
+      </c>
+      <c r="AD57" s="2" t="s">
+        <v>4508</v>
+      </c>
+      <c r="AE57" s="2" t="s">
+        <v>4509</v>
+      </c>
+      <c r="AF57" s="2" t="s">
+        <v>4510</v>
+      </c>
+      <c r="AG57" s="2" t="s">
+        <v>4511</v>
+      </c>
+      <c r="AH57" s="2" t="s">
+        <v>2833</v>
+      </c>
+      <c r="AI57" s="2" t="s">
+        <v>2834</v>
       </c>
       <c r="AJ57" s="1" t="s">
         <v>2887</v>
@@ -23282,10 +24857,76 @@
       <c r="BC57" s="1" t="s">
         <v>3118</v>
       </c>
+      <c r="BF57" s="2" t="s">
+        <v>4698</v>
+      </c>
     </row>
-    <row r="58" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI58" s="1" t="s">
-        <v>2830</v>
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N58" s="2" t="s">
+        <v>4420</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>4421</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>4512</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>4513</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>4514</v>
+      </c>
+      <c r="S58" s="2" t="s">
+        <v>4515</v>
+      </c>
+      <c r="T58" s="2" t="s">
+        <v>4516</v>
+      </c>
+      <c r="U58" s="2" t="s">
+        <v>4517</v>
+      </c>
+      <c r="V58" s="2" t="s">
+        <v>4518</v>
+      </c>
+      <c r="W58" s="2" t="s">
+        <v>4519</v>
+      </c>
+      <c r="X58" s="2" t="s">
+        <v>4520</v>
+      </c>
+      <c r="Y58" s="2" t="s">
+        <v>4521</v>
+      </c>
+      <c r="Z58" s="2" t="s">
+        <v>4522</v>
+      </c>
+      <c r="AA58" s="2" t="s">
+        <v>4523</v>
+      </c>
+      <c r="AB58" s="2" t="s">
+        <v>4524</v>
+      </c>
+      <c r="AC58" s="2" t="s">
+        <v>4525</v>
+      </c>
+      <c r="AD58" s="2" t="s">
+        <v>4526</v>
+      </c>
+      <c r="AE58" s="2" t="s">
+        <v>4527</v>
+      </c>
+      <c r="AF58" s="2" t="s">
+        <v>4528</v>
+      </c>
+      <c r="AG58" s="2" t="s">
+        <v>4529</v>
+      </c>
+      <c r="AH58" s="2" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AI58" s="2" t="s">
+        <v>2836</v>
       </c>
       <c r="AJ58" s="1" t="s">
         <v>2889</v>
@@ -23347,10 +24988,18 @@
       <c r="BC58" s="1" t="s">
         <v>3136</v>
       </c>
+      <c r="BF58" s="2" t="s">
+        <v>4699</v>
+      </c>
     </row>
-    <row r="59" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI59" s="1" t="s">
-        <v>2831</v>
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="AH59" s="2" t="s">
+        <v>2837</v>
+      </c>
+      <c r="AI59" s="2" t="s">
+        <v>2838</v>
       </c>
       <c r="AJ59" s="1" t="s">
         <v>2891</v>
@@ -23412,10 +25061,18 @@
       <c r="BC59" s="1" t="s">
         <v>3154</v>
       </c>
+      <c r="BF59" s="2" t="s">
+        <v>4700</v>
+      </c>
     </row>
-    <row r="60" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI60" s="1" t="s">
-        <v>2832</v>
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="AH60" s="2" t="s">
+        <v>2839</v>
+      </c>
+      <c r="AI60" s="2" t="s">
+        <v>2840</v>
       </c>
       <c r="AJ60" s="1" t="s">
         <v>2893</v>
@@ -23477,10 +25134,18 @@
       <c r="BC60" s="1" t="s">
         <v>3172</v>
       </c>
+      <c r="BF60" s="2" t="s">
+        <v>4701</v>
+      </c>
     </row>
-    <row r="61" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI61" s="1" t="s">
-        <v>2833</v>
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="AH61" s="2" t="s">
+        <v>2841</v>
+      </c>
+      <c r="AI61" s="2" t="s">
+        <v>2842</v>
       </c>
       <c r="AJ61" s="1" t="s">
         <v>2895</v>
@@ -23542,10 +25207,18 @@
       <c r="BC61" s="1" t="s">
         <v>3190</v>
       </c>
+      <c r="BF61" s="2" t="s">
+        <v>4702</v>
+      </c>
     </row>
-    <row r="62" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI62" s="1" t="s">
-        <v>2834</v>
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="AH62" s="2" t="s">
+        <v>2843</v>
+      </c>
+      <c r="AI62" s="2" t="s">
+        <v>2844</v>
       </c>
       <c r="AJ62" s="1" t="s">
         <v>2897</v>
@@ -23607,10 +25280,18 @@
       <c r="BC62" s="1" t="s">
         <v>3208</v>
       </c>
+      <c r="BF62" s="2" t="s">
+        <v>4703</v>
+      </c>
     </row>
-    <row r="63" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI63" s="1" t="s">
-        <v>2835</v>
+    <row r="63" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="AH63" s="2" t="s">
+        <v>2845</v>
+      </c>
+      <c r="AI63" s="2" t="s">
+        <v>2846</v>
       </c>
       <c r="AJ63" s="1" t="s">
         <v>2899</v>
@@ -23672,10 +25353,18 @@
       <c r="BC63" s="1" t="s">
         <v>3226</v>
       </c>
+      <c r="BF63" s="2" t="s">
+        <v>4704</v>
+      </c>
     </row>
-    <row r="64" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AI64" s="1" t="s">
-        <v>2836</v>
+    <row r="64" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="AH64" s="2" t="s">
+        <v>2847</v>
+      </c>
+      <c r="AI64" s="2" t="s">
+        <v>2848</v>
       </c>
       <c r="AJ64" s="1" t="s">
         <v>2901</v>
@@ -23737,10 +25426,16 @@
       <c r="BC64" s="1" t="s">
         <v>3244</v>
       </c>
+      <c r="BF64" s="2" t="s">
+        <v>4705</v>
+      </c>
     </row>
-    <row r="65" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI65" s="1" t="s">
-        <v>2837</v>
+    <row r="65" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH65" s="2" t="s">
+        <v>2849</v>
+      </c>
+      <c r="AI65" s="2" t="s">
+        <v>2850</v>
       </c>
       <c r="AJ65" s="1" t="s">
         <v>2903</v>
@@ -23802,10 +25497,16 @@
       <c r="BC65" s="1" t="s">
         <v>3262</v>
       </c>
+      <c r="BF65" s="2" t="s">
+        <v>4706</v>
+      </c>
     </row>
-    <row r="66" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI66" s="1" t="s">
-        <v>2838</v>
+    <row r="66" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH66" s="2" t="s">
+        <v>2851</v>
+      </c>
+      <c r="AI66" s="2" t="s">
+        <v>2852</v>
       </c>
       <c r="AJ66" s="1" t="s">
         <v>2905</v>
@@ -23867,10 +25568,16 @@
       <c r="BC66" s="1" t="s">
         <v>3280</v>
       </c>
+      <c r="BF66" s="2" t="s">
+        <v>4707</v>
+      </c>
     </row>
-    <row r="67" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI67" s="1" t="s">
-        <v>2839</v>
+    <row r="67" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH67" s="2" t="s">
+        <v>2853</v>
+      </c>
+      <c r="AI67" s="2" t="s">
+        <v>2854</v>
       </c>
       <c r="AJ67" s="1" t="s">
         <v>2907</v>
@@ -23932,10 +25639,16 @@
       <c r="BC67" s="1" t="s">
         <v>3298</v>
       </c>
+      <c r="BF67" s="2" t="s">
+        <v>4708</v>
+      </c>
     </row>
-    <row r="68" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI68" s="1" t="s">
-        <v>2840</v>
+    <row r="68" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH68" s="2" t="s">
+        <v>2855</v>
+      </c>
+      <c r="AI68" s="2" t="s">
+        <v>2856</v>
       </c>
       <c r="AJ68" s="1" t="s">
         <v>2909</v>
@@ -23997,10 +25710,16 @@
       <c r="BC68" s="1" t="s">
         <v>3316</v>
       </c>
+      <c r="BF68" s="2" t="s">
+        <v>4709</v>
+      </c>
     </row>
-    <row r="69" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI69" s="1" t="s">
-        <v>2841</v>
+    <row r="69" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH69" s="2" t="s">
+        <v>2857</v>
+      </c>
+      <c r="AI69" s="2" t="s">
+        <v>2858</v>
       </c>
       <c r="AJ69" s="1" t="s">
         <v>2911</v>
@@ -24062,10 +25781,16 @@
       <c r="BC69" s="1" t="s">
         <v>3334</v>
       </c>
+      <c r="BF69" s="2" t="s">
+        <v>4710</v>
+      </c>
     </row>
-    <row r="70" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI70" s="1" t="s">
-        <v>2842</v>
+    <row r="70" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH70" s="2" t="s">
+        <v>2859</v>
+      </c>
+      <c r="AI70" s="2" t="s">
+        <v>2860</v>
       </c>
       <c r="AJ70" s="1" t="s">
         <v>2913</v>
@@ -24127,10 +25852,16 @@
       <c r="BC70" s="1" t="s">
         <v>3352</v>
       </c>
+      <c r="BF70" s="2" t="s">
+        <v>4711</v>
+      </c>
     </row>
-    <row r="71" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI71" s="1" t="s">
-        <v>2843</v>
+    <row r="71" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH71" s="2" t="s">
+        <v>2861</v>
+      </c>
+      <c r="AI71" s="2" t="s">
+        <v>2862</v>
       </c>
       <c r="AJ71" s="1" t="s">
         <v>2915</v>
@@ -24192,10 +25923,16 @@
       <c r="BC71" s="1" t="s">
         <v>3370</v>
       </c>
+      <c r="BF71" s="2" t="s">
+        <v>4712</v>
+      </c>
     </row>
-    <row r="72" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI72" s="1" t="s">
-        <v>2844</v>
+    <row r="72" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH72" s="2" t="s">
+        <v>2863</v>
+      </c>
+      <c r="AI72" s="2" t="s">
+        <v>2864</v>
       </c>
       <c r="AJ72" s="1" t="s">
         <v>2917</v>
@@ -24257,10 +25994,16 @@
       <c r="BC72" s="1" t="s">
         <v>3388</v>
       </c>
+      <c r="BF72" s="2" t="s">
+        <v>4713</v>
+      </c>
     </row>
-    <row r="73" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI73" s="1" t="s">
-        <v>2845</v>
+    <row r="73" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH73" s="2" t="s">
+        <v>2865</v>
+      </c>
+      <c r="AI73" s="2" t="s">
+        <v>2866</v>
       </c>
       <c r="AJ73" s="1" t="s">
         <v>2919</v>
@@ -24322,10 +26065,16 @@
       <c r="BC73" s="1" t="s">
         <v>3406</v>
       </c>
+      <c r="BF73" s="2" t="s">
+        <v>4714</v>
+      </c>
     </row>
-    <row r="74" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI74" s="1" t="s">
-        <v>2846</v>
+    <row r="74" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH74" s="2" t="s">
+        <v>2867</v>
+      </c>
+      <c r="AI74" s="2" t="s">
+        <v>2868</v>
       </c>
       <c r="AJ74" s="1" t="s">
         <v>2921</v>
@@ -24387,10 +26136,16 @@
       <c r="BC74" s="1" t="s">
         <v>3424</v>
       </c>
+      <c r="BF74" s="2" t="s">
+        <v>4715</v>
+      </c>
     </row>
-    <row r="75" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI75" s="1" t="s">
-        <v>2847</v>
+    <row r="75" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH75" s="2" t="s">
+        <v>2869</v>
+      </c>
+      <c r="AI75" s="2" t="s">
+        <v>2870</v>
       </c>
       <c r="AJ75" s="1" t="s">
         <v>2923</v>
@@ -24452,10 +26207,16 @@
       <c r="BC75" s="1" t="s">
         <v>3442</v>
       </c>
+      <c r="BF75" s="2" t="s">
+        <v>4716</v>
+      </c>
     </row>
-    <row r="76" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI76" s="1" t="s">
-        <v>2848</v>
+    <row r="76" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH76" s="2" t="s">
+        <v>2871</v>
+      </c>
+      <c r="AI76" s="2" t="s">
+        <v>2872</v>
       </c>
       <c r="AJ76" s="1" t="s">
         <v>2925</v>
@@ -24517,10 +26278,16 @@
       <c r="BC76" s="1" t="s">
         <v>3460</v>
       </c>
+      <c r="BF76" s="2" t="s">
+        <v>4717</v>
+      </c>
     </row>
-    <row r="77" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI77" s="1" t="s">
-        <v>2849</v>
+    <row r="77" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH77" s="2" t="s">
+        <v>2873</v>
+      </c>
+      <c r="AI77" s="2" t="s">
+        <v>2874</v>
       </c>
       <c r="AJ77" s="1" t="s">
         <v>2927</v>
@@ -24582,10 +26349,16 @@
       <c r="BC77" s="1" t="s">
         <v>3478</v>
       </c>
+      <c r="BF77" s="2" t="s">
+        <v>4718</v>
+      </c>
     </row>
-    <row r="78" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI78" s="1" t="s">
-        <v>2850</v>
+    <row r="78" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH78" s="2" t="s">
+        <v>2875</v>
+      </c>
+      <c r="AI78" s="2" t="s">
+        <v>2876</v>
       </c>
       <c r="AJ78" s="1" t="s">
         <v>2929</v>
@@ -24647,10 +26420,16 @@
       <c r="BC78" s="1" t="s">
         <v>3496</v>
       </c>
+      <c r="BF78" s="2" t="s">
+        <v>4719</v>
+      </c>
     </row>
-    <row r="79" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI79" s="1" t="s">
-        <v>2851</v>
+    <row r="79" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH79" s="2" t="s">
+        <v>2877</v>
+      </c>
+      <c r="AI79" s="2" t="s">
+        <v>2878</v>
       </c>
       <c r="AJ79" s="1" t="s">
         <v>2931</v>
@@ -24712,10 +26491,16 @@
       <c r="BC79" s="1" t="s">
         <v>3514</v>
       </c>
+      <c r="BF79" s="2" t="s">
+        <v>4720</v>
+      </c>
     </row>
-    <row r="80" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI80" s="1" t="s">
-        <v>2852</v>
+    <row r="80" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH80" s="2" t="s">
+        <v>4530</v>
+      </c>
+      <c r="AI80" s="2" t="s">
+        <v>4531</v>
       </c>
       <c r="AJ80" s="1" t="s">
         <v>2933</v>
@@ -24777,10 +26562,16 @@
       <c r="BC80" s="1" t="s">
         <v>3532</v>
       </c>
+      <c r="BF80" s="2" t="s">
+        <v>4721</v>
+      </c>
     </row>
-    <row r="81" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI81" s="1" t="s">
-        <v>2853</v>
+    <row r="81" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH81" s="2" t="s">
+        <v>4532</v>
+      </c>
+      <c r="AI81" s="2" t="s">
+        <v>4533</v>
       </c>
       <c r="AJ81" s="1" t="s">
         <v>2935</v>
@@ -24842,10 +26633,16 @@
       <c r="BC81" s="1" t="s">
         <v>3550</v>
       </c>
+      <c r="BF81" s="2" t="s">
+        <v>4722</v>
+      </c>
     </row>
-    <row r="82" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI82" s="1" t="s">
-        <v>2854</v>
+    <row r="82" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH82" s="2" t="s">
+        <v>4534</v>
+      </c>
+      <c r="AI82" s="2" t="s">
+        <v>4535</v>
       </c>
       <c r="AJ82" s="1" t="s">
         <v>2937</v>
@@ -24907,10 +26704,16 @@
       <c r="BC82" s="1" t="s">
         <v>3568</v>
       </c>
+      <c r="BF82" s="2" t="s">
+        <v>4723</v>
+      </c>
     </row>
-    <row r="83" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI83" s="1" t="s">
-        <v>2855</v>
+    <row r="83" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH83" s="2" t="s">
+        <v>4536</v>
+      </c>
+      <c r="AI83" s="2" t="s">
+        <v>4537</v>
       </c>
       <c r="AJ83" s="1" t="s">
         <v>2939</v>
@@ -24972,10 +26775,16 @@
       <c r="BC83" s="1" t="s">
         <v>3586</v>
       </c>
+      <c r="BF83" s="2" t="s">
+        <v>4724</v>
+      </c>
     </row>
-    <row r="84" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI84" s="1" t="s">
-        <v>2856</v>
+    <row r="84" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH84" s="2" t="s">
+        <v>4538</v>
+      </c>
+      <c r="AI84" s="2" t="s">
+        <v>4539</v>
       </c>
       <c r="AJ84" s="1" t="s">
         <v>2941</v>
@@ -25037,10 +26846,16 @@
       <c r="BC84" s="1" t="s">
         <v>3604</v>
       </c>
+      <c r="BF84" s="2" t="s">
+        <v>4725</v>
+      </c>
     </row>
-    <row r="85" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI85" s="1" t="s">
-        <v>2857</v>
+    <row r="85" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH85" s="2" t="s">
+        <v>4540</v>
+      </c>
+      <c r="AI85" s="2" t="s">
+        <v>4541</v>
       </c>
       <c r="AJ85" s="1" t="s">
         <v>2943</v>
@@ -25102,10 +26917,16 @@
       <c r="BC85" s="1" t="s">
         <v>3622</v>
       </c>
+      <c r="BF85" s="2" t="s">
+        <v>4726</v>
+      </c>
     </row>
-    <row r="86" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI86" s="1" t="s">
-        <v>2858</v>
+    <row r="86" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH86" s="2" t="s">
+        <v>4542</v>
+      </c>
+      <c r="AI86" s="2" t="s">
+        <v>4543</v>
       </c>
       <c r="AJ86" s="1" t="s">
         <v>2945</v>
@@ -25167,10 +26988,16 @@
       <c r="BC86" s="1" t="s">
         <v>3640</v>
       </c>
+      <c r="BF86" s="2" t="s">
+        <v>4727</v>
+      </c>
     </row>
-    <row r="87" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI87" s="1" t="s">
-        <v>2859</v>
+    <row r="87" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH87" s="2" t="s">
+        <v>4544</v>
+      </c>
+      <c r="AI87" s="2" t="s">
+        <v>4545</v>
       </c>
       <c r="AJ87" s="1" t="s">
         <v>2947</v>
@@ -25232,10 +27059,16 @@
       <c r="BC87" s="1" t="s">
         <v>3658</v>
       </c>
+      <c r="BF87" s="2" t="s">
+        <v>4728</v>
+      </c>
     </row>
-    <row r="88" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI88" s="1" t="s">
-        <v>2860</v>
+    <row r="88" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH88" s="2" t="s">
+        <v>4546</v>
+      </c>
+      <c r="AI88" s="2" t="s">
+        <v>4547</v>
       </c>
       <c r="AJ88" s="1" t="s">
         <v>2949</v>
@@ -25297,10 +27130,16 @@
       <c r="BC88" s="1" t="s">
         <v>3676</v>
       </c>
+      <c r="BF88" s="2" t="s">
+        <v>4729</v>
+      </c>
     </row>
-    <row r="89" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI89" s="1" t="s">
-        <v>2861</v>
+    <row r="89" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH89" s="2" t="s">
+        <v>4548</v>
+      </c>
+      <c r="AI89" s="2" t="s">
+        <v>4549</v>
       </c>
       <c r="AJ89" s="1" t="s">
         <v>2951</v>
@@ -25362,10 +27201,16 @@
       <c r="BC89" s="1" t="s">
         <v>3694</v>
       </c>
+      <c r="BF89" s="2" t="s">
+        <v>4730</v>
+      </c>
     </row>
-    <row r="90" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI90" s="1" t="s">
-        <v>2862</v>
+    <row r="90" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH90" s="2" t="s">
+        <v>4550</v>
+      </c>
+      <c r="AI90" s="2" t="s">
+        <v>4551</v>
       </c>
       <c r="AJ90" s="1" t="s">
         <v>2953</v>
@@ -25427,10 +27272,16 @@
       <c r="BC90" s="1" t="s">
         <v>3712</v>
       </c>
+      <c r="BF90" s="2" t="s">
+        <v>4731</v>
+      </c>
     </row>
-    <row r="91" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI91" s="1" t="s">
-        <v>2863</v>
+    <row r="91" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH91" s="2" t="s">
+        <v>4552</v>
+      </c>
+      <c r="AI91" s="2" t="s">
+        <v>4553</v>
       </c>
       <c r="AJ91" s="1" t="s">
         <v>2955</v>
@@ -25492,10 +27343,16 @@
       <c r="BC91" s="1" t="s">
         <v>3730</v>
       </c>
+      <c r="BF91" s="2" t="s">
+        <v>4732</v>
+      </c>
     </row>
-    <row r="92" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI92" s="1" t="s">
-        <v>2864</v>
+    <row r="92" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH92" s="2" t="s">
+        <v>4554</v>
+      </c>
+      <c r="AI92" s="2" t="s">
+        <v>4555</v>
       </c>
       <c r="AJ92" s="1" t="s">
         <v>2957</v>
@@ -25557,10 +27414,16 @@
       <c r="BC92" s="1" t="s">
         <v>3748</v>
       </c>
+      <c r="BF92" s="2" t="s">
+        <v>4733</v>
+      </c>
     </row>
-    <row r="93" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI93" s="1" t="s">
-        <v>2865</v>
+    <row r="93" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH93" s="2" t="s">
+        <v>4556</v>
+      </c>
+      <c r="AI93" s="2" t="s">
+        <v>4557</v>
       </c>
       <c r="AJ93" s="1" t="s">
         <v>2959</v>
@@ -25622,10 +27485,16 @@
       <c r="BC93" s="1" t="s">
         <v>3766</v>
       </c>
+      <c r="BF93" s="2" t="s">
+        <v>4734</v>
+      </c>
     </row>
-    <row r="94" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI94" s="1" t="s">
-        <v>2866</v>
+    <row r="94" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH94" s="2" t="s">
+        <v>4558</v>
+      </c>
+      <c r="AI94" s="2" t="s">
+        <v>4559</v>
       </c>
       <c r="AJ94" s="1" t="s">
         <v>2961</v>
@@ -25687,10 +27556,16 @@
       <c r="BC94" s="1" t="s">
         <v>3784</v>
       </c>
+      <c r="BF94" s="2" t="s">
+        <v>4735</v>
+      </c>
     </row>
-    <row r="95" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI95" s="1" t="s">
-        <v>2867</v>
+    <row r="95" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH95" s="2" t="s">
+        <v>4560</v>
+      </c>
+      <c r="AI95" s="2" t="s">
+        <v>4561</v>
       </c>
       <c r="AJ95" s="1" t="s">
         <v>2963</v>
@@ -25752,10 +27627,16 @@
       <c r="BC95" s="1" t="s">
         <v>3802</v>
       </c>
+      <c r="BF95" s="2" t="s">
+        <v>4736</v>
+      </c>
     </row>
-    <row r="96" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI96" s="1" t="s">
-        <v>2868</v>
+    <row r="96" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH96" s="2" t="s">
+        <v>4562</v>
+      </c>
+      <c r="AI96" s="2" t="s">
+        <v>4563</v>
       </c>
       <c r="AJ96" s="1" t="s">
         <v>2965</v>
@@ -25817,10 +27698,16 @@
       <c r="BC96" s="1" t="s">
         <v>3820</v>
       </c>
+      <c r="BF96" s="2" t="s">
+        <v>4737</v>
+      </c>
     </row>
-    <row r="97" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI97" s="1" t="s">
-        <v>2869</v>
+    <row r="97" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH97" s="2" t="s">
+        <v>4564</v>
+      </c>
+      <c r="AI97" s="2" t="s">
+        <v>4565</v>
       </c>
       <c r="AJ97" s="1" t="s">
         <v>2967</v>
@@ -25882,10 +27769,16 @@
       <c r="BC97" s="1" t="s">
         <v>3838</v>
       </c>
+      <c r="BF97" s="2" t="s">
+        <v>4738</v>
+      </c>
     </row>
-    <row r="98" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI98" s="1" t="s">
-        <v>2870</v>
+    <row r="98" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH98" s="2" t="s">
+        <v>4566</v>
+      </c>
+      <c r="AI98" s="2" t="s">
+        <v>4567</v>
       </c>
       <c r="AJ98" s="1" t="s">
         <v>2969</v>
@@ -25947,10 +27840,16 @@
       <c r="BC98" s="1" t="s">
         <v>3856</v>
       </c>
+      <c r="BF98" s="2" t="s">
+        <v>4739</v>
+      </c>
     </row>
-    <row r="99" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI99" s="1" t="s">
-        <v>2871</v>
+    <row r="99" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH99" s="2" t="s">
+        <v>4568</v>
+      </c>
+      <c r="AI99" s="2" t="s">
+        <v>4569</v>
       </c>
       <c r="AJ99" s="1" t="s">
         <v>2971</v>
@@ -26012,10 +27911,16 @@
       <c r="BC99" s="1" t="s">
         <v>3874</v>
       </c>
+      <c r="BF99" s="2" t="s">
+        <v>4740</v>
+      </c>
     </row>
-    <row r="100" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI100" s="1" t="s">
-        <v>2872</v>
+    <row r="100" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH100" s="2" t="s">
+        <v>4570</v>
+      </c>
+      <c r="AI100" s="2" t="s">
+        <v>4571</v>
       </c>
       <c r="AJ100" s="1" t="s">
         <v>2973</v>
@@ -26077,10 +27982,16 @@
       <c r="BC100" s="1" t="s">
         <v>3892</v>
       </c>
+      <c r="BF100" s="2" t="s">
+        <v>4741</v>
+      </c>
     </row>
-    <row r="101" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI101" s="1" t="s">
-        <v>2873</v>
+    <row r="101" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH101" s="2" t="s">
+        <v>4572</v>
+      </c>
+      <c r="AI101" s="2" t="s">
+        <v>4573</v>
       </c>
       <c r="AJ101" s="1" t="s">
         <v>2975</v>
@@ -26142,10 +28053,16 @@
       <c r="BC101" s="1" t="s">
         <v>3910</v>
       </c>
+      <c r="BF101" s="2" t="s">
+        <v>4742</v>
+      </c>
     </row>
-    <row r="102" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI102" s="1" t="s">
-        <v>2874</v>
+    <row r="102" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH102" s="2" t="s">
+        <v>4574</v>
+      </c>
+      <c r="AI102" s="2" t="s">
+        <v>4575</v>
       </c>
       <c r="AJ102" s="1" t="s">
         <v>2977</v>
@@ -26207,10 +28124,16 @@
       <c r="BC102" s="1" t="s">
         <v>3928</v>
       </c>
+      <c r="BF102" s="2" t="s">
+        <v>4743</v>
+      </c>
     </row>
-    <row r="103" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI103" s="1" t="s">
-        <v>2875</v>
+    <row r="103" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH103" s="2" t="s">
+        <v>4576</v>
+      </c>
+      <c r="AI103" s="2" t="s">
+        <v>4577</v>
       </c>
       <c r="AJ103" s="1" t="s">
         <v>2979</v>
@@ -26273,9 +28196,12 @@
         <v>3946</v>
       </c>
     </row>
-    <row r="104" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI104" s="1" t="s">
-        <v>2876</v>
+    <row r="104" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH104" s="2" t="s">
+        <v>4578</v>
+      </c>
+      <c r="AI104" s="2" t="s">
+        <v>4579</v>
       </c>
       <c r="AJ104" s="1" t="s">
         <v>2981</v>
@@ -26338,9 +28264,12 @@
         <v>3964</v>
       </c>
     </row>
-    <row r="105" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI105" s="1" t="s">
-        <v>2877</v>
+    <row r="105" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH105" s="2" t="s">
+        <v>4580</v>
+      </c>
+      <c r="AI105" s="2" t="s">
+        <v>4581</v>
       </c>
       <c r="AJ105" s="1" t="s">
         <v>2983</v>
@@ -26403,9 +28332,12 @@
         <v>3982</v>
       </c>
     </row>
-    <row r="106" spans="35:55" x14ac:dyDescent="0.25">
-      <c r="AI106" s="1" t="s">
-        <v>2878</v>
+    <row r="106" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH106" s="2" t="s">
+        <v>4582</v>
+      </c>
+      <c r="AI106" s="2" t="s">
+        <v>4583</v>
       </c>
       <c r="AJ106" s="1" t="s">
         <v>2985</v>
@@ -26468,7 +28400,13 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="107" spans="35:55" x14ac:dyDescent="0.25">
+    <row r="107" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH107" s="2" t="s">
+        <v>4584</v>
+      </c>
+      <c r="AI107" s="2" t="s">
+        <v>4585</v>
+      </c>
       <c r="AJ107" s="1" t="s">
         <v>2987</v>
       </c>
@@ -26530,7 +28468,13 @@
         <v>4018</v>
       </c>
     </row>
-    <row r="108" spans="35:55" x14ac:dyDescent="0.25">
+    <row r="108" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH108" s="2" t="s">
+        <v>4586</v>
+      </c>
+      <c r="AI108" s="2" t="s">
+        <v>4587</v>
+      </c>
       <c r="AJ108" s="1" t="s">
         <v>2989</v>
       </c>
@@ -26592,7 +28536,13 @@
         <v>4036</v>
       </c>
     </row>
-    <row r="109" spans="35:55" x14ac:dyDescent="0.25">
+    <row r="109" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH109" s="2" t="s">
+        <v>4588</v>
+      </c>
+      <c r="AI109" s="2" t="s">
+        <v>4589</v>
+      </c>
       <c r="AJ109" s="1" t="s">
         <v>2991</v>
       </c>
@@ -26654,7 +28604,13 @@
         <v>4054</v>
       </c>
     </row>
-    <row r="110" spans="35:55" x14ac:dyDescent="0.25">
+    <row r="110" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH110" s="2" t="s">
+        <v>4590</v>
+      </c>
+      <c r="AI110" s="2" t="s">
+        <v>4591</v>
+      </c>
       <c r="AJ110" s="1" t="s">
         <v>2993</v>
       </c>
@@ -26716,7 +28672,13 @@
         <v>4072</v>
       </c>
     </row>
-    <row r="111" spans="35:55" x14ac:dyDescent="0.25">
+    <row r="111" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH111" s="2" t="s">
+        <v>4592</v>
+      </c>
+      <c r="AI111" s="2" t="s">
+        <v>4593</v>
+      </c>
       <c r="AJ111" s="1" t="s">
         <v>2995</v>
       </c>
@@ -26778,7 +28740,13 @@
         <v>4090</v>
       </c>
     </row>
-    <row r="112" spans="35:55" x14ac:dyDescent="0.25">
+    <row r="112" spans="34:58" x14ac:dyDescent="0.25">
+      <c r="AH112" s="2" t="s">
+        <v>4594</v>
+      </c>
+      <c r="AI112" s="2" t="s">
+        <v>4595</v>
+      </c>
       <c r="AJ112" s="1" t="s">
         <v>2997</v>
       </c>
@@ -26840,7 +28808,13 @@
         <v>4108</v>
       </c>
     </row>
-    <row r="113" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="113" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH113" s="2" t="s">
+        <v>4596</v>
+      </c>
+      <c r="AI113" s="2" t="s">
+        <v>4597</v>
+      </c>
       <c r="AJ113" s="1" t="s">
         <v>2999</v>
       </c>
@@ -26902,7 +28876,13 @@
         <v>4126</v>
       </c>
     </row>
-    <row r="114" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="114" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH114" s="2" t="s">
+        <v>4598</v>
+      </c>
+      <c r="AI114" s="2" t="s">
+        <v>4599</v>
+      </c>
       <c r="AJ114" s="1" t="s">
         <v>3001</v>
       </c>
@@ -26964,7 +28944,13 @@
         <v>4144</v>
       </c>
     </row>
-    <row r="115" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="115" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH115" s="2" t="s">
+        <v>4600</v>
+      </c>
+      <c r="AI115" s="2" t="s">
+        <v>4601</v>
+      </c>
       <c r="AJ115" s="1" t="s">
         <v>3003</v>
       </c>
@@ -27026,7 +29012,13 @@
         <v>4162</v>
       </c>
     </row>
-    <row r="116" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="116" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH116" s="2" t="s">
+        <v>4602</v>
+      </c>
+      <c r="AI116" s="2" t="s">
+        <v>4603</v>
+      </c>
       <c r="AJ116" s="1" t="s">
         <v>3005</v>
       </c>
@@ -27088,7 +29080,13 @@
         <v>4180</v>
       </c>
     </row>
-    <row r="117" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="117" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH117" s="2" t="s">
+        <v>4604</v>
+      </c>
+      <c r="AI117" s="2" t="s">
+        <v>4605</v>
+      </c>
       <c r="AJ117" s="1" t="s">
         <v>3007</v>
       </c>
@@ -27150,7 +29148,13 @@
         <v>4198</v>
       </c>
     </row>
-    <row r="118" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="118" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH118" s="2" t="s">
+        <v>4606</v>
+      </c>
+      <c r="AI118" s="2" t="s">
+        <v>4607</v>
+      </c>
       <c r="AJ118" s="1" t="s">
         <v>3009</v>
       </c>
@@ -27212,7 +29216,13 @@
         <v>4216</v>
       </c>
     </row>
-    <row r="119" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="119" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH119" s="2" t="s">
+        <v>4608</v>
+      </c>
+      <c r="AI119" s="2" t="s">
+        <v>4609</v>
+      </c>
       <c r="AJ119" s="1" t="s">
         <v>3011</v>
       </c>
@@ -27274,7 +29284,13 @@
         <v>4234</v>
       </c>
     </row>
-    <row r="120" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="120" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH120" s="2" t="s">
+        <v>4610</v>
+      </c>
+      <c r="AI120" s="2" t="s">
+        <v>4611</v>
+      </c>
       <c r="AJ120" s="1" t="s">
         <v>3013</v>
       </c>
@@ -27336,7 +29352,13 @@
         <v>4252</v>
       </c>
     </row>
-    <row r="121" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="121" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH121" s="2" t="s">
+        <v>4612</v>
+      </c>
+      <c r="AI121" s="2" t="s">
+        <v>4613</v>
+      </c>
       <c r="AJ121" s="1" t="s">
         <v>3015</v>
       </c>
@@ -27398,7 +29420,13 @@
         <v>4270</v>
       </c>
     </row>
-    <row r="122" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="122" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH122" s="2" t="s">
+        <v>4614</v>
+      </c>
+      <c r="AI122" s="2" t="s">
+        <v>4615</v>
+      </c>
       <c r="AJ122" s="1" t="s">
         <v>3017</v>
       </c>
@@ -27460,7 +29488,13 @@
         <v>4288</v>
       </c>
     </row>
-    <row r="123" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="123" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH123" s="2" t="s">
+        <v>4616</v>
+      </c>
+      <c r="AI123" s="2" t="s">
+        <v>4617</v>
+      </c>
       <c r="AJ123" s="1" t="s">
         <v>3019</v>
       </c>
@@ -27522,7 +29556,13 @@
         <v>4306</v>
       </c>
     </row>
-    <row r="124" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="124" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH124" s="2" t="s">
+        <v>4618</v>
+      </c>
+      <c r="AI124" s="2" t="s">
+        <v>4619</v>
+      </c>
       <c r="AJ124" s="1" t="s">
         <v>3021</v>
       </c>
@@ -27584,7 +29624,13 @@
         <v>4324</v>
       </c>
     </row>
-    <row r="125" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="125" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH125" s="2" t="s">
+        <v>4620</v>
+      </c>
+      <c r="AI125" s="2" t="s">
+        <v>4621</v>
+      </c>
       <c r="AJ125" s="1" t="s">
         <v>3023</v>
       </c>
@@ -27646,7 +29692,13 @@
         <v>4342</v>
       </c>
     </row>
-    <row r="126" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="126" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH126" s="2" t="s">
+        <v>4622</v>
+      </c>
+      <c r="AI126" s="2" t="s">
+        <v>4623</v>
+      </c>
       <c r="AJ126" s="1" t="s">
         <v>3025</v>
       </c>
@@ -27708,7 +29760,13 @@
         <v>4360</v>
       </c>
     </row>
-    <row r="127" spans="36:55" x14ac:dyDescent="0.25">
+    <row r="127" spans="34:55" x14ac:dyDescent="0.25">
+      <c r="AH127" s="2" t="s">
+        <v>4624</v>
+      </c>
+      <c r="AI127" s="2" t="s">
+        <v>4625</v>
+      </c>
       <c r="AJ127" s="1" t="s">
         <v>3027</v>
       </c>

</xml_diff>

<commit_message>
U-pick implementation. Improved sorting robustness.
</commit_message>
<xml_diff>
--- a/_LAYOUT.xlsx
+++ b/_LAYOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\BinSortSequence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6B1B08-84EF-4D94-A6BB-2BAE379DDE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479B903C-96C0-4116-8CC6-65C64FA711A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WAREHOUSE_LAYOUT" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4858" uniqueCount="4750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4862" uniqueCount="4754">
   <si>
     <t>01-001-1</t>
   </si>
@@ -14285,6 +14285,18 @@
   </si>
   <si>
     <t>8040-003</t>
+  </si>
+  <si>
+    <t>AisleUPick#</t>
+  </si>
+  <si>
+    <t>U-pick pattern sorting of # length in ascending order</t>
+  </si>
+  <si>
+    <t>U-pick pattern sorting of # length in descending order</t>
+  </si>
+  <si>
+    <t>AisleReverseUPick#</t>
   </si>
 </sst>
 </file>
@@ -15159,7 +15171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -30788,10 +30800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEB32EA-3168-4C84-A276-945E883034DE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30840,6 +30852,22 @@
         <v>2814</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4750</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4753</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4752</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>